<commit_message>
Implementation of the security and authentication functionality.
</commit_message>
<xml_diff>
--- a/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
+++ b/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="LOKACIJA" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,11 @@
     <sheet name="NOMENKALTURA_SPORTOVA" sheetId="8" r:id="rId7"/>
     <sheet name="VREDNOVANJE_DEFINICIJA_UPITNIKA" sheetId="9" r:id="rId8"/>
     <sheet name="VREDNOVANJE_VRIJEDNOSTI_PITANJA" sheetId="10" r:id="rId9"/>
+    <sheet name="USERS" sheetId="11" r:id="rId10"/>
+    <sheet name="AUTHORITIES" sheetId="12" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BANK_ACCOUNT!$A$1:$D$163</definedName>
@@ -152,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="1807">
   <si>
     <t>RBR</t>
   </si>
@@ -5543,6 +5545,36 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>ENABLED</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>$2a$04$PGghSlPUBJtDCs8pMXrj0OAbJN3deO1FVUKcgheGuyQgnMN65lx5m</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>USER ID</t>
+  </si>
+  <si>
+    <t>ROLE_USER</t>
+  </si>
+  <si>
+    <t>ROLE_ADMIN</t>
   </si>
 </sst>
 </file>
@@ -5770,7 +5802,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5856,6 +5888,7 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6265,12 +6298,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="28" t="str">
+        <f>"insert into diskobolos.users(username, password, email, enabled) values ('"&amp;A2&amp;"', '"&amp;B2&amp;"',  '"&amp;C2&amp;"',  "&amp;D2&amp;");"</f>
+        <v>insert into diskobolos.users(username, password, email, enabled) values ('test', '$2a$04$PGghSlPUBJtDCs8pMXrj0OAbJN3deO1FVUKcgheGuyQgnMN65lx5m',  'test@gmail.com',  TRUE);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="28" t="str">
+        <f>"insert into diskobolos.authorities(role, user_id) values ('"&amp;A2&amp;"',  "&amp;B2&amp;");"</f>
+        <v>insert into diskobolos.authorities(role, user_id) values ('ROLE_USER',  1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="28" t="str">
+        <f>"insert into diskobolos.authorities(role, user_id) values ('"&amp;A3&amp;"',  "&amp;B3&amp;");"</f>
+        <v>insert into diskobolos.authorities(role, user_id) values ('ROLE_ADMIN',  1);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6375,6 +6514,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20857,7 +20997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Displaying informations about currently logged user.
</commit_message>
<xml_diff>
--- a/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
+++ b/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="1807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1808">
   <si>
     <t>RBR</t>
   </si>
@@ -5575,6 +5575,9 @@
   </si>
   <si>
     <t>ROLE_ADMIN</t>
+  </si>
+  <si>
+    <t>PERMISSION_LEVEL</t>
   </si>
 </sst>
 </file>
@@ -6353,49 +6356,59 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>1803</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>1804</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C1" s="35" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>1805</v>
       </c>
       <c r="B2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="str">
-        <f>"insert into diskobolos.authorities(role, user_id) values ('"&amp;A2&amp;"',  "&amp;B2&amp;");"</f>
-        <v>insert into diskobolos.authorities(role, user_id) values ('ROLE_USER',  1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C2" s="15">
+        <v>2</v>
+      </c>
+      <c r="E2" s="28" t="str">
+        <f>"insert into diskobolos.authorities(role, user_id, permission_level) values ('"&amp;A2&amp;"',  "&amp;B2&amp;", "&amp;C2&amp;");"</f>
+        <v>insert into diskobolos.authorities(role, user_id, permission_level) values ('ROLE_USER',  1, 2);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1806</v>
       </c>
       <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="str">
-        <f>"insert into diskobolos.authorities(role, user_id) values ('"&amp;A3&amp;"',  "&amp;B3&amp;");"</f>
-        <v>insert into diskobolos.authorities(role, user_id) values ('ROLE_ADMIN',  1);</v>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="28" t="str">
+        <f>"insert into diskobolos.authorities(role, user_id, permission_level) values ('"&amp;A3&amp;"',  "&amp;B3&amp;", "&amp;C3&amp;");"</f>
+        <v>insert into diskobolos.authorities(role, user_id, permission_level) values ('ROLE_ADMIN',  1, 0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sport categories are added into the member register spreadsheet (excel)
</commit_message>
<xml_diff>
--- a/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
+++ b/complete/src/main/java/scripts/sql/resources/Prepared data for the DB.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr backupFile="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tommy\Documents\NetBeansProjects\DiskobolosCore\complete\src\main\java\scripts\sql\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pro\Documents\NetBeansProjects\DiskobolosCore\complete\src\main\java\scripts\sql\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LOKACIJA" sheetId="2" r:id="rId1"/>
@@ -49,6 +49,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tommy čax</author>
+    <author>Pro</author>
   </authors>
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0">
@@ -149,12 +150,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q63" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="1960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="1962">
   <si>
     <t>RBR</t>
   </si>
@@ -6034,6 +6059,12 @@
   </si>
   <si>
     <t>ZRAKOPLOVSTVO</t>
+  </si>
+  <si>
+    <t>KATEGORIJA SPORTA</t>
+  </si>
+  <si>
+    <t>OSTALO</t>
   </si>
 </sst>
 </file>
@@ -6184,7 +6215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -6261,6 +6292,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -6268,7 +6323,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6352,6 +6407,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10814,10 +10887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R160"/>
+  <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="B157" workbookViewId="0">
+      <selection activeCell="Q155" sqref="Q155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10827,9 +10900,10 @@
     <col min="3" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -10878,8 +10952,11 @@
       <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -10926,12 +11003,15 @@
       <c r="P2" s="6">
         <v>1</v>
       </c>
-      <c r="R2" s="3" t="str">
+      <c r="Q2" s="40" t="s">
+        <v>1762</v>
+      </c>
+      <c r="S2" s="3" t="str">
         <f>"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B2&amp;"',  "&amp;C2&amp;", '"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"', '"&amp;H2&amp;"','"&amp;I2&amp;"', '"&amp;J2&amp;"', '"&amp;K2&amp;"', '"&amp;L2&amp;"',to_date(NULLIF('"&amp;IF(M2="","",M2)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N2="","",N2)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O2="","",O2)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P2&amp;"');"</f>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Aikido klub Zadar',  1, '023/251-210','','023/251-210','3639975', '35182939735','13000118', '0073359', 'Nenad Vertovšek (091/337-77-76)', 'Vesna Vertovšek (091/512-65-87)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -10975,15 +11055,18 @@
       <c r="O3" s="4" t="s">
         <v>1615</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="39">
         <v>1</v>
       </c>
-      <c r="R3" s="3" t="str">
-        <f t="shared" ref="R3:R66" si="0">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B3&amp;"',  "&amp;C3&amp;", '"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"', '"&amp;H3&amp;"','"&amp;I3&amp;"', '"&amp;J3&amp;"', '"&amp;K3&amp;"', '"&amp;L3&amp;"',to_date(NULLIF('"&amp;IF(M3="","",M3)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N3="","",N3)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O3="","",O3)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P3&amp;"');"</f>
+      <c r="Q3" s="41" t="s">
+        <v>1763</v>
+      </c>
+      <c r="S3" s="3" t="str">
+        <f t="shared" ref="S3:S66" si="0">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B3&amp;"',  "&amp;C3&amp;", '"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"', '"&amp;H3&amp;"','"&amp;I3&amp;"', '"&amp;J3&amp;"', '"&amp;K3&amp;"', '"&amp;L3&amp;"',to_date(NULLIF('"&amp;IF(M3="","",M3)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N3="","",N3)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O3="","",O3)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P3&amp;"');"</f>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Atletski športski klub Zadar',  2, '023/301-691','','023/301-691','03154912', '86624179675','13000308', '01128100', 'Emilijo Krstić (098/721-876)', 'Helena Vulić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -11026,12 +11109,15 @@
       <c r="P4" s="2">
         <v>1</v>
       </c>
-      <c r="R4" s="3" t="str">
+      <c r="Q4" s="38" t="s">
+        <v>1762</v>
+      </c>
+      <c r="S4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski aikido klub Donat',  3, '','','','02411423', '40633085803','13001042', '0086495', 'Renata Ruić Funčić  (091/539-24-92)', 'Goran Funčić  (091/539-24-91)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -11078,12 +11164,15 @@
       <c r="P5" s="2">
         <v>1</v>
       </c>
-      <c r="R5" s="3" t="str">
+      <c r="Q5" s="37" t="s">
+        <v>1763</v>
+      </c>
+      <c r="S5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Atletski klub Alojzije Stepinac',  4, '023/326-109','','023/326-109','02013517', '35240858683','13000826', '0200101', 'Mladen Peša', 'Gabrijela Miolović (098/133-70-36)',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -11130,12 +11219,15 @@
       <c r="P6" s="2">
         <v>1</v>
       </c>
-      <c r="R6" s="3" t="str">
+      <c r="Q6" s="37" t="s">
+        <v>1763</v>
+      </c>
+      <c r="S6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Atletski klub Olympionik',  5, '023/213-899','','023/213-899','02464551', '57024317058','13001078', '0250249', 'Perica Korica (098/330 - 257)', 'Petar Korica (091/161-11-66)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -11182,12 +11274,15 @@
       <c r="P7" s="2">
         <v>1</v>
       </c>
-      <c r="R7" s="3" t="str">
+      <c r="Q7" s="37" t="s">
+        <v>1763</v>
+      </c>
+      <c r="S7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Atletski klub Start',  6, '023/315-523','','023/315-523','02791889', '36113911509','13001326', '0247539', 'Jurica Vuleta  (098/935-2793)', 'Ivan Mijolović',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -11230,12 +11325,15 @@
       <c r="P8" s="2">
         <v>1</v>
       </c>
-      <c r="R8" s="3" t="str">
+      <c r="Q8" s="37" t="s">
+        <v>1763</v>
+      </c>
+      <c r="S8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub atletskih veterana Zadar',  7, '','','','01930117', '02457723462','13000778', '0198958', 'Borislav Perica (098/909-51-62)', 'Danijel Tadić (098/196-86-70)',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -11278,12 +11376,15 @@
       <c r="P9" s="2">
         <v>1</v>
       </c>
-      <c r="R9" s="3" t="str">
+      <c r="Q9" s="37" t="s">
+        <v>1759</v>
+      </c>
+      <c r="S9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Automobilistički klub ZD tuning',  8, '','','','02434571', '07178578094','13001059', '0189089', 'Toni Perinić (095/525-88-19)', 'Jure Perić: (091/598-05-99)',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -11328,12 +11429,15 @@
       <c r="P10" s="2">
         <v>1</v>
       </c>
-      <c r="R10" s="3" t="str">
+      <c r="Q10" s="37" t="s">
+        <v>1758</v>
+      </c>
+      <c r="S10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Badminton klub Iader',  9, '023/240-406','','','02570211', '85070743078','13001162', '0263324', 'Ernesto Šimac  (099/317-79-62)', 'Mario Murtić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -11380,12 +11484,15 @@
       <c r="P11" s="2">
         <v>1</v>
       </c>
-      <c r="R11" s="3" t="str">
+      <c r="Q11" s="37" t="s">
+        <v>1756</v>
+      </c>
+      <c r="S11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Baseball klub Donat',  10, '023/7305-409','','023/319-075','03414264', '10554665928','13000422', '0017507', 'Ivica Anić  (098/853 - 869)', 'Zoran Šijan (098/366 - 673)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -11430,12 +11537,15 @@
       <c r="P12" s="2">
         <v>1</v>
       </c>
-      <c r="R12" s="3" t="str">
+      <c r="Q12" s="37" t="s">
+        <v>1754</v>
+      </c>
+      <c r="S12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Biciklistički klub Sv. Donat',  11, '023/315-632','','','01560913', '23423721111','13000210', '0217834', 'Denis Šepat', 'Ivan Krpina (095/199-19-45)',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -11480,12 +11590,15 @@
       <c r="P13" s="2">
         <v>1</v>
       </c>
-      <c r="R13" s="3" t="str">
+      <c r="Q13" s="37" t="s">
+        <v>1754</v>
+      </c>
+      <c r="S13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Biciklistički klub Zadar',  12, '023/315-632','','','03154882', '80916067371','13000315', '0136826', 'Božidar Kotlar', 'Neven Pavić  (098/177-18-01)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -11530,12 +11643,15 @@
       <c r="P14" s="2">
         <v>1</v>
       </c>
-      <c r="R14" s="3" t="str">
+      <c r="Q14" s="42" t="s">
+        <v>1754</v>
+      </c>
+      <c r="S14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Biciklistički klub Macaklin',  13, '023/342-190','','','02480018', '21483252848','13001060', '0189521', 'Ivan Govorčin (095/900-83-08)', 'Daniel Filić (091/893-62-37)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('19.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>14</v>
       </c>
@@ -11582,12 +11698,15 @@
       <c r="P15" s="2">
         <v>1</v>
       </c>
-      <c r="R15" s="3" t="str">
+      <c r="Q15" s="37" t="s">
+        <v>1753</v>
+      </c>
+      <c r="S15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Biljar klub 11',  14, '023/324-118','','0123/312-235','2194295', '76378932354','13000911', '0342154', 'Čedomir Perinčić ( 098/463-552)', 'Iva Perinčić',to_date(NULLIF('01.01.2001', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2005', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -11634,12 +11753,15 @@
       <c r="P16" s="2">
         <v>1</v>
       </c>
-      <c r="R16" s="3" t="str">
+      <c r="Q16" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski klub Bili Brig',  15, '023/327-957','','023/327-957','03450848', '53640895488','13000381', '0217137', 'Goran Lijić (091/449-2922)', 'Zdenko Stipanić (098/950-73-32)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>16</v>
       </c>
@@ -11686,12 +11808,15 @@
       <c r="P17" s="2">
         <v>1</v>
       </c>
-      <c r="R17" s="3" t="str">
+      <c r="Q17" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski klub Brodarica',  16, '023/332-487','','023/332-487','03933644', '03283371919','13000205', '0306770', 'Jozo Jeličić (098/192-00-08)', 'Željko Sabalić (098/192-00-08)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -11734,12 +11859,15 @@
       <c r="P18" s="2">
         <v>1</v>
       </c>
-      <c r="R18" s="3" t="str">
+      <c r="Q18" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski klub Veteran',  17, '023/333-174','','','03418618', '69602095812','13000471', '', 'Luka Škara (092/306-40-96)', 'Marjan Nimac (098/449-819)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -11784,12 +11912,15 @@
       <c r="P19" s="2">
         <v>1</v>
       </c>
-      <c r="R19" s="3" t="str">
+      <c r="Q19" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski klub Zadar',  18, '023/214-093','','023/214-093','03450848', 'O3836929990','13000253', '', 'Milivoj Colić (098/196-27-65)', 'Šime Burerin (091/789-78-64)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -11830,12 +11961,15 @@
       <c r="P20" s="2">
         <v>1</v>
       </c>
-      <c r="R20" s="3" t="str">
+      <c r="Q20" s="37" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski klub Crvene kuće',  19, '','','','02631920', '11984817013','13001207', '0216999', 'Ante Kardum (095/903-1759)', '',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -11882,12 +12016,15 @@
       <c r="P21" s="2">
         <v>1</v>
       </c>
-      <c r="R21" s="3" t="str">
+      <c r="Q21" s="42" t="s">
+        <v>1749</v>
+      </c>
+      <c r="S21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boksački klub Diabolik',  20, '023/241-334','','023/241-334','00711233', '62256903451','13000342', '0128898', 'Damir Zrilić (098/643-238)', 'Mario Pešut (098/332-844)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>21</v>
       </c>
@@ -11932,12 +12069,15 @@
       <c r="P22" s="2">
         <v>1</v>
       </c>
-      <c r="R22" s="3" t="str">
+      <c r="Q22" s="37" t="s">
+        <v>1749</v>
+      </c>
+      <c r="S22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boksački klub Zadar',  21, '099/7637493','','','03173887', '14313344538','13000235', '0121468', 'Dragan Vidaić (099/76-37-493)', 'Branka Vidaić (098/888-585)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>22</v>
       </c>
@@ -11984,12 +12124,15 @@
       <c r="P23" s="2">
         <v>1</v>
       </c>
-      <c r="R23" s="3" t="str">
+      <c r="Q23" s="37" t="s">
+        <v>1749</v>
+      </c>
+      <c r="S23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Jedriličarski klub Uskok',  22, '023/337-830','','023/333-888','03154840', '18816234272','13000046', '0121468', 'Ive Mustać (098/207-269)', 'Hrvoje Grdović (099/529-37-84)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>23</v>
       </c>
@@ -12036,12 +12179,15 @@
       <c r="P24" s="2">
         <v>1</v>
       </c>
-      <c r="R24" s="3" t="str">
+      <c r="Q24" s="37" t="s">
+        <v>1881</v>
+      </c>
+      <c r="S24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Judo klub Zadar',  23, '023/324-984','','023/324-984','00824682', '14954453186','13000050', '0042102', 'Ante Zanki (098/332-584)', 'Irena Zanki (099/214-88-33)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>24</v>
       </c>
@@ -12088,12 +12234,15 @@
       <c r="P25" s="2">
         <v>1</v>
       </c>
-      <c r="R25" s="3" t="str">
+      <c r="Q25" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Jazine - Arbanasi',  24, '023/213-214','','023/224-488','0317585', '00054311768','13000210', '0137133', 'Branko Morić (098/730-042)', 'Miljan Ćustić (091/976-77-40)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>25</v>
       </c>
@@ -12136,12 +12285,15 @@
       <c r="P26" s="2">
         <v>1</v>
       </c>
-      <c r="R26" s="3" t="str">
+      <c r="Q26" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Zadar š.d.d.',  25, '023/212-441','','023/212-441','03154955', '9051939443','', '', 'Boris Skroče (091/508-51-14)', 'Vana Dundov (098/415-598)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>26</v>
       </c>
@@ -12188,12 +12340,15 @@
       <c r="P27" s="2">
         <v>1</v>
       </c>
-      <c r="R27" s="3" t="str">
+      <c r="Q27" s="37" t="s">
+        <v>1896</v>
+      </c>
+      <c r="S27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kuglački klub Donat zaštita',  26, '023/493-845','','023/493-845','01565362', '26478293512','13000526', '0189372', 'Marin Colić (091/528-93-33)', 'Jakov Krstić',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>27</v>
       </c>
@@ -12240,12 +12395,15 @@
       <c r="P28" s="2">
         <v>1</v>
       </c>
-      <c r="R28" s="3" t="str">
+      <c r="Q28" s="37" t="s">
+        <v>1896</v>
+      </c>
+      <c r="S28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kuglački klub Zadar',  27, '023/240-122','','023/240-120','03197735', '59524922370','13000117', '0094625', 'Ivan Lulić (098/981-69-00)', 'Marija Lulić',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>28</v>
       </c>
@@ -12288,12 +12446,15 @@
       <c r="P29" s="2">
         <v>1</v>
       </c>
-      <c r="R29" s="3" t="str">
+      <c r="Q29" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Nogometni klub Zadar š.d.d.',  28, '023/312-792','','023/312-802','04295030', '06621814362','', '', 'Josip Bajlo (091/530-44-66)', 'Mladen Baždarić (098/378-792)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>29</v>
       </c>
@@ -12338,12 +12499,15 @@
       <c r="P30" s="2">
         <v>1</v>
       </c>
-      <c r="R30" s="3" t="str">
+      <c r="Q30" s="37" t="s">
+        <v>1909</v>
+      </c>
+      <c r="S30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Odbojkaški klub Zadar',  29, '023/213-809','','023/213-403','03154777', '60567527217','13000241', '0073709', 'Robert Kresoja (098/330-231)', '',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>30</v>
       </c>
@@ -12390,12 +12554,15 @@
       <c r="P31" s="2">
         <v>1</v>
       </c>
-      <c r="R31" s="3" t="str">
+      <c r="Q31" s="37" t="s">
+        <v>1913</v>
+      </c>
+      <c r="S31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Planinarsko društvo Paklenica',  30, '023/301-636','','023/301-636','03154939', '92966614510','13000356', '0124394', 'Domagoj Diklić (099/213-12-22)', 'Vesna Dukić',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>31</v>
       </c>
@@ -12442,12 +12609,15 @@
       <c r="P32" s="2">
         <v>1</v>
       </c>
-      <c r="R32" s="3" t="str">
+      <c r="Q32" s="37" t="s">
+        <v>1916</v>
+      </c>
+      <c r="S32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Plivački klub Zadar',  31, '023/312-320','','023/312-320','03429644', '83018458598','13000252', '0162874', 'Darko Smirkinić (098/331-057)', 'Anja Jelinić (099/803-85-21)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>32</v>
       </c>
@@ -12494,12 +12664,15 @@
       <c r="P33" s="2">
         <v>1</v>
       </c>
-      <c r="R33" s="3" t="str">
+      <c r="Q33" s="37" t="s">
+        <v>1922</v>
+      </c>
+      <c r="S33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ronilački klub "KPA"',  32, '023/332-954','','023/332-954','03154831', '43628357665','13000343', '0016918', 'Slavica Čolak (098/184-22-14)', 'Marija Velemir (099/341-72-25)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>33</v>
       </c>
@@ -12546,12 +12719,15 @@
       <c r="P34" s="2">
         <v>1</v>
       </c>
-      <c r="R34" s="3" t="str">
+      <c r="Q34" s="37" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Stolnoteniski klub Donat',  33, '023/242-096','','023/242-096','03155072', '51868892731','13000322', '0086614', 'Davor Aras (098/214-215)', 'Ljubomir Letinić (091/886-56-12)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>34</v>
       </c>
@@ -12598,12 +12774,15 @@
       <c r="P35" s="2">
         <v>1</v>
       </c>
-      <c r="R35" s="3" t="str">
+      <c r="Q35" s="37" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Streljački klub Zadar',  34, '023/331-050','','023/331-050','03155048', '14707241415','13000309', '0125660', 'Jadranko Surać (098/499-334)', 'Davor Zubčić (098/226-139)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>35</v>
       </c>
@@ -12648,12 +12827,15 @@
       <c r="P36" s="2">
         <v>1</v>
       </c>
-      <c r="R36" s="3" t="str">
+      <c r="Q36" s="37" t="s">
+        <v>1944</v>
+      </c>
+      <c r="S36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Šahovski klub Zadar',  35, '023/251-632','','','03154998', '74633093402','13000232', '0163733', 'Josip Bubičić (098/968-79-99)', 'Krolo (098/734-388)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>36</v>
       </c>
@@ -12700,16 +12882,19 @@
       <c r="P37" s="2">
         <v>1</v>
       </c>
-      <c r="R37" s="3" t="str">
+      <c r="Q37" s="37" t="s">
+        <v>1948</v>
+      </c>
+      <c r="S37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športsko ribolovno društvo Zubatac',  36, '023/212-708','','023/214-441','03159922', '90755644642','13000341', '0120681', 'Ardena Bajlo (091/207-25-35)', 'Branko Šuljak (091/225-11-29)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>394</v>
       </c>
       <c r="C38" s="17">
@@ -12742,12 +12927,15 @@
       <c r="P38" s="2">
         <v>1</v>
       </c>
-      <c r="R38" s="3" t="str">
+      <c r="Q38" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ordinacija Športske medicine',  37, '023/334-859','','023/334-859','80067247', '30089337645','', '', 'Doktor: dr. Marko Prenđa (091/125-02-32)', '',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>38</v>
       </c>
@@ -12794,12 +12982,15 @@
       <c r="P39" s="2">
         <v>1</v>
       </c>
-      <c r="R39" s="3" t="str">
+      <c r="Q39" s="37" t="s">
+        <v>1953</v>
+      </c>
+      <c r="S39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Teniski klub Zadar 08',  38, '023/334-859','','023/334-859','03151492', '65605226586','13000168', '0164423', 'Lovro Rončević (098/172-0228)', 'Albert Radovniković (098/160-71-37)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>39</v>
       </c>
@@ -12842,12 +13033,15 @@
       <c r="P40" s="2">
         <v>1</v>
       </c>
-      <c r="R40" s="3" t="str">
+      <c r="Q40" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga za šport i rekreaciju invalida Grada Zadra',  39, '023/333-477','','023/323-400','01230131', '82239066808','', '', 'Ivica Bratanović (099/509-67-65)', 'Ivan Anušić (098/191-24-60)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>40</v>
       </c>
@@ -12894,12 +13088,15 @@
       <c r="P41" s="2">
         <v>1</v>
       </c>
-      <c r="R41" s="3" t="str">
+      <c r="Q41" s="37" t="s">
+        <v>1957</v>
+      </c>
+      <c r="S41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Veslački klub Jadran',  40, '023/316-929','','023/316-929','03154807', '48176749093','13000303', '0073717', 'Klaudijo Stipčević (091/750-20-77)', 'Darija Kraljević (098/734-374)',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>41</v>
       </c>
@@ -12940,12 +13137,15 @@
       <c r="P42" s="2">
         <v>1</v>
       </c>
-      <c r="R42" s="3" t="str">
+      <c r="Q42" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Javna ustanova za upravljanje športskim objektima - Zadarski šport d.o.o.',  41, '023/331-197','','023/331-400','1366432', '98185775176','', '', 'Direktor: Jurica Dilber (091/591-19-77)', '',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>42</v>
       </c>
@@ -12992,12 +13192,15 @@
       <c r="P43" s="2">
         <v>1</v>
       </c>
-      <c r="R43" s="3" t="str">
+      <c r="Q43" s="37" t="s">
+        <v>1923</v>
+      </c>
+      <c r="S43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ženski rukometni klub Zadar',  42, '023/341-034','','023/342-630','03154971', '35599539345','13000306', '0151330', 'Dražen Dajak (091/204-04-40)', 'Nela Mitrović (098/191-29-61)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>43</v>
       </c>
@@ -13042,12 +13245,15 @@
       <c r="P44" s="2">
         <v>1</v>
       </c>
-      <c r="R44" s="3" t="str">
+      <c r="Q44" s="37" t="s">
+        <v>1946</v>
+      </c>
+      <c r="S44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski plesni klub Samba',  43, '023/312-518','','','01443615', '66124427579','13000395', '0097063', 'Zlatka Badel (098/650-873', 'Bernarda Kaurloto',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>44</v>
       </c>
@@ -13092,12 +13298,15 @@
       <c r="P45" s="2">
         <v>1</v>
       </c>
-      <c r="R45" s="3" t="str">
+      <c r="Q45" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Diklo',  44, '023/337-038','','023/337-064','01619144', '59710612309','13000575', '0041793', 'Verino Ladiš (097/715-9866)', '',to_date(NULLIF('01.01.2007', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>45</v>
       </c>
@@ -13144,12 +13353,15 @@
       <c r="P46" s="2">
         <v>1</v>
       </c>
-      <c r="R46" s="3" t="str">
+      <c r="Q46" s="37" t="s">
+        <v>1922</v>
+      </c>
+      <c r="S46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ronilaćki klub Zadar',  45, '023/324-306','','023/324-306','01564005', '73191012166','13000534', '0132341', 'Duško Paulin (091/4848-588)', 'Vjekoslav Valčić (091/7306-39-69)',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>46</v>
       </c>
@@ -13196,12 +13408,15 @@
       <c r="P47" s="2">
         <v>1</v>
       </c>
-      <c r="R47" s="3" t="str">
+      <c r="Q47" s="37" t="s">
+        <v>1939</v>
+      </c>
+      <c r="S47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Stolnoteniski klub Jadera',  46, '023/250-020','','023/250-020','02433826', '69211850445','13001070', '0112305', 'Ivica Bujas (099/599-16-97)', 'Mario Kožul (091/508-98-33)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>47</v>
       </c>
@@ -13246,12 +13461,15 @@
       <c r="P48" s="2">
         <v>1</v>
       </c>
-      <c r="R48" s="3" t="str">
+      <c r="Q48" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Voštarnica',  47, '023/326-176','','','01717081', '21803934153','13000661', '0188686', 'Tomislav Klarica (091/326-17-66)', 'Igor Dorontić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>48</v>
       </c>
@@ -13296,12 +13514,15 @@
       <c r="P49" s="2">
         <v>1</v>
       </c>
-      <c r="R49" s="3" t="str">
+      <c r="Q49" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Nogometni Klub Arbanasi',  48, '023/311-759','','','01815598', '48701891138','13000727', '0120746', 'Edi Perović', 'Miodrag PAunović (091/733-46-06)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>49</v>
       </c>
@@ -13346,12 +13567,15 @@
       <c r="P50" s="2">
         <v>1</v>
       </c>
-      <c r="R50" s="3" t="str">
+      <c r="Q50" s="42" t="s">
+        <v>1886</v>
+      </c>
+      <c r="S50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Karate klub Croatia',  49, '023/319-014','','023/250-048','03587967', '68920650220','13000152', '0041696', 'Hrvoje Mikecin (091/760-49-66)', '',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>50</v>
       </c>
@@ -13398,12 +13622,15 @@
       <c r="P51" s="2">
         <v>1</v>
       </c>
-      <c r="R51" s="3" t="str">
+      <c r="Q51" s="37" t="s">
+        <v>1916</v>
+      </c>
+      <c r="S51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Plivački klub Jadera',  50, '023/334-933','','023/334-933','02230518', '80828570466','13000943', '0041831', 'Vitomir Burčul (098/166-01-13)', 'Marijan Čulina (098/976-35-23)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>51</v>
       </c>
@@ -13446,12 +13673,15 @@
       <c r="P52" s="2">
         <v>1</v>
       </c>
-      <c r="R52" s="3" t="str">
+      <c r="Q52" s="37" t="s">
+        <v>1954</v>
+      </c>
+      <c r="S52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Triatlon klub Zadar',  51, '','','','02564343', '79243095913','13001164', '0151891', 'Ivan Gobin (098/180-54-34)', 'Ivan Tuta (098/180-54-34)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>52</v>
       </c>
@@ -13498,12 +13728,15 @@
       <c r="P53" s="2">
         <v>1</v>
       </c>
-      <c r="R53" s="3" t="str">
+      <c r="Q53" s="37" t="s">
+        <v>1951</v>
+      </c>
+      <c r="S53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Taekwondo klub Zadar',  52, '023/302-374','','023/302-374','03439330', '18649423025','1300032', '0127916', 'Mladen Uskok (098/303-311)', 'Krešimir Karamarko (099/311-49-17)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>53</v>
       </c>
@@ -13546,12 +13779,15 @@
       <c r="P54" s="2">
         <v>1</v>
       </c>
-      <c r="R54" s="3" t="str">
+      <c r="Q54" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Pet bunara - veterani',  53, '','','','02823071', '57896242721','13001345', '0198799', 'Tonći Jerak (099/882-26-23)', 'Jure Jerak (091/348-07-37)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>54</v>
       </c>
@@ -13598,12 +13834,15 @@
       <c r="P55" s="2">
         <v>1</v>
       </c>
-      <c r="R55" s="3" t="str">
+      <c r="Q55" s="37" t="s">
+        <v>1923</v>
+      </c>
+      <c r="S55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Rukometni klub Zadar 1954',  54, '023/34-772','','023/324-772','01856979', '39778663780','13000745', '0149344', 'Rade Šimićević  (098/98-464)', 'Igor Nikolić (098/944-48-00)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>55</v>
       </c>
@@ -13650,12 +13889,15 @@
       <c r="P56" s="2">
         <v>1</v>
       </c>
-      <c r="R56" s="3" t="str">
+      <c r="Q56" s="37" t="s">
+        <v>1886</v>
+      </c>
+      <c r="S56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Karate klub Zvonimir',  55, '023/311-552','','023/311-552','02201844', '06972084253','13000932', '0085588', 'Tomislav Rogić (098/614-413)', 'Franjp Glavaš (098/614-413)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>56</v>
       </c>
@@ -13698,12 +13940,15 @@
       <c r="P57" s="2">
         <v>1</v>
       </c>
-      <c r="R57" s="3" t="str">
+      <c r="Q57" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Višnjik',  56, '023/231-551','','023/231-551','01799746', '19104518057','130007000', '0271499', 'Ivica Jukić (095/198-12-43)', 'Matija Benini (095/914-89-69)',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>57</v>
       </c>
@@ -13750,12 +13995,15 @@
       <c r="P58" s="2">
         <v>1</v>
       </c>
-      <c r="R58" s="3" t="str">
+      <c r="Q58" s="37" t="s">
+        <v>1896</v>
+      </c>
+      <c r="S58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kuglački klub Donat Zadar - Žene',  57, '023/334-811 ','023/351-504','','03189082', '22505058872','13000338', '0103128', 'Ante Lonić (099/572-71-86)', 'Nives Grabovac (098/248-379) Žaklina Jelača (091/788-47-68)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>58</v>
       </c>
@@ -13802,12 +14050,15 @@
       <c r="P59" s="2">
         <v>1</v>
       </c>
-      <c r="R59" s="3" t="str">
+      <c r="Q59" s="37" t="s">
+        <v>1875</v>
+      </c>
+      <c r="S59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub ritmičke gimnastike Sirena',  58, '023/340-531','','023/340-531','02412411', '91916030955','13001049', '0116012', 'Iris Mijailović Bulj (095/830-50-70)', 'Irena Serdarević',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>59</v>
       </c>
@@ -13852,12 +14103,15 @@
       <c r="P60" s="2">
         <v>1</v>
       </c>
-      <c r="R60" s="3" t="str">
+      <c r="Q60" s="37" t="s">
+        <v>1759</v>
+      </c>
+      <c r="S60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Automobilistički klub RTZ',  59, '','','023/778-895','02626209', '62512974921','13001198', '0218241', 'Goran Ban (095/808-47-75)', 'Iva Borošak',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>60</v>
       </c>
@@ -13900,12 +14154,15 @@
       <c r="P61" s="2">
         <v>1</v>
       </c>
-      <c r="R61" s="3" t="str">
+      <c r="Q61" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo Športske rekreacije Vitalnost',  60, '','','','02549336', '89335027474','13001140', '01011959', 'Ivana Stilinović (098/903-46-17)', 'Filip Simičić',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>61</v>
       </c>
@@ -13952,12 +14209,15 @@
       <c r="P62" s="2">
         <v>1</v>
       </c>
-      <c r="R62" s="3" t="str">
+      <c r="Q62" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub ABC',  61, '023/326-176','','023/326-176','01462016', '50180654492','13000415', '0128093', 'Željko Pribanović (091/326-35-35)', 'Davor Rosan',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>62</v>
       </c>
@@ -14000,12 +14260,15 @@
       <c r="P63" s="2">
         <v>1</v>
       </c>
-      <c r="R63" s="3" t="str">
+      <c r="Q63" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športska škola košarke Zadar',  62, '023/230-750','','023/230-750','02273454', '80406652845','130400116', '0028584', 'Tonći Jerak (099/311-16-47)', 'Zdenko Perić',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>63</v>
       </c>
@@ -14052,12 +14315,15 @@
       <c r="P64" s="2">
         <v>1</v>
       </c>
-      <c r="R64" s="3" t="str">
+      <c r="Q64" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga za mali nogomet Zadarske županije',  63, '023/314-521','','023/254-180','03417255', '09849416974','13000182', '0151224', 'Zvonimir Sorić (098/272-525)', 'Matetrbušić (095/889-46-93)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>64</v>
       </c>
@@ -14100,12 +14366,15 @@
       <c r="P65" s="2">
         <v>1</v>
       </c>
-      <c r="R65" s="3" t="str">
+      <c r="Q65" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Futsal',  64, '023/321-361','','023/321-361','02936470', '23999408148','', '0265341', 'Marko Šimurina (091/515-51-52)', '',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>65</v>
       </c>
@@ -14148,12 +14417,15 @@
       <c r="P66" s="2">
         <v>1</v>
       </c>
-      <c r="R66" s="3" t="str">
+      <c r="Q66" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Puntamika',  65, '','','','01669435', '47719025627','13000628', '0151020', 'Alan Kociper (098/180-60-12)', 'Stela Dunić',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>66</v>
       </c>
@@ -14196,12 +14468,15 @@
       <c r="P67" s="2">
         <v>1</v>
       </c>
-      <c r="R67" s="3" t="str">
-        <f t="shared" ref="R67:R130" si="1">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B67&amp;"',  "&amp;C67&amp;", '"&amp;D67&amp;"','"&amp;E67&amp;"','"&amp;F67&amp;"','"&amp;G67&amp;"', '"&amp;H67&amp;"','"&amp;I67&amp;"', '"&amp;J67&amp;"', '"&amp;K67&amp;"', '"&amp;L67&amp;"',to_date(NULLIF('"&amp;IF(M67="","",M67)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N67="","",N67)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O67="","",O67)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P67&amp;"');"</f>
+      <c r="Q67" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S67" s="3" t="str">
+        <f t="shared" ref="S67:S130" si="1">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B67&amp;"',  "&amp;C67&amp;", '"&amp;D67&amp;"','"&amp;E67&amp;"','"&amp;F67&amp;"','"&amp;G67&amp;"', '"&amp;H67&amp;"','"&amp;I67&amp;"', '"&amp;J67&amp;"', '"&amp;K67&amp;"', '"&amp;L67&amp;"',to_date(NULLIF('"&amp;IF(M67="","",M67)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N67="","",N67)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O67="","",O67)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P67&amp;"');"</f>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športsko rekreacijska udruga Sklek',  66, '023/326-682','','','02301644', '09909070165','13000983', '0150518', 'Vedrana Pleslić (095/909-3525)', '',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>67</v>
       </c>
@@ -14244,12 +14519,15 @@
       <c r="P68" s="2">
         <v>1</v>
       </c>
-      <c r="R68" s="3" t="str">
+      <c r="Q68" s="37" t="s">
+        <v>1940</v>
+      </c>
+      <c r="S68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Streličarski klub Zadar',  67, '','','','02671816', '65872367322','13001218', '0168838', 'Irena Stein (098/817-065)', 'Maja Pavković (098/315-082)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>68</v>
       </c>
@@ -14290,12 +14568,15 @@
       <c r="P69" s="2">
         <v>1</v>
       </c>
-      <c r="R69" s="3" t="str">
+      <c r="Q69" s="37" t="s">
+        <v>1921</v>
+      </c>
+      <c r="S69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ragbi klub Zadar',  68, '023/305-428','','','02234645', '93943012649','13000926', '0189992', 'Mateo Mazija (091/201-45-83)', 'Radošević Ivan (091/957-46-18)',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>69</v>
       </c>
@@ -14342,12 +14623,15 @@
       <c r="P70" s="2">
         <v>1</v>
       </c>
-      <c r="R70" s="3" t="str">
+      <c r="Q70" s="37" t="s">
+        <v>1956</v>
+      </c>
+      <c r="S70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Vaterpolski klub Zadar 1952',  69, '023/237-614','','023/206-898','01675826', '33644431140','13000637', '0190617', 'Dražen Grgurović (098/981-69-00)', 'Goran Jovančević (099/323-15-62)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>70</v>
       </c>
@@ -14394,12 +14678,15 @@
       <c r="P71" s="2">
         <v>1</v>
       </c>
-      <c r="R71" s="3" t="str">
+      <c r="Q71" s="37" t="s">
+        <v>1875</v>
+      </c>
+      <c r="S71" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Gimnastički klub Salto',  70, '023/236-384','','023/350-390','02228416', '165952126666','13000939', '0041904', 'Marko Sutlović (099/255-77-70)', 'Ivana Ratković (099/813-44-31)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>71</v>
       </c>
@@ -14446,12 +14733,15 @@
       <c r="P72" s="2">
         <v>1</v>
       </c>
-      <c r="R72" s="3" t="str">
+      <c r="Q72" s="42" t="s">
+        <v>1944</v>
+      </c>
+      <c r="S72" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Šahovski klub Casper',  71, '023/312-794','','023/254-020','01264818', '39897562507','13000236', '0112361', 'Veljko Šagi (091/170-21-40)', 'Margita Gurdulić',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>72</v>
       </c>
@@ -14498,12 +14788,15 @@
       <c r="P73" s="2">
         <v>1</v>
       </c>
-      <c r="R73" s="3" t="str">
+      <c r="Q73" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S73" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Silba',  72, '023/323-861','','023/323-861','02331357', '09726047291','13000985', '0192857', 'Ante Žorrž (098/198-48-62)', 'Marko Žorž (095/902-04-80)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>73</v>
       </c>
@@ -14534,12 +14827,15 @@
       <c r="P74" s="2">
         <v>1</v>
       </c>
-      <c r="R74" s="3" t="str">
+      <c r="Q74" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S74" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Drakmar Sali',  73, '','','','', '97831826928','', '', 'Šanto Basioli (099/833-83-97)', '',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>74</v>
       </c>
@@ -14586,12 +14882,15 @@
       <c r="P75" s="2">
         <v>1</v>
       </c>
-      <c r="R75" s="3" t="str">
+      <c r="Q75" s="37" t="s">
+        <v>1679</v>
+      </c>
+      <c r="S75" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Županijski savez školskog športa Zadarske županije',  74, '023/312-289','','023/312-289','01661132', '44327231995','13000606', '0041572', 'Davor Vidaković (098/332-874)', 'Jadranka Duvančić (091/207-24-02)',to_date(NULLIF('05.11.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('05.11.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>75</v>
       </c>
@@ -14638,12 +14937,15 @@
       <c r="P76" s="2">
         <v>1</v>
       </c>
-      <c r="R76" s="3" t="str">
+      <c r="Q76" s="37" t="s">
+        <v>1913</v>
+      </c>
+      <c r="S76" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Hrvatsko planinarsko društvo Mala Rava',  75, '023/333-681','','023/333-681','02635640', '22514563488','13001204', '0188441', 'Zoran Simičić (095/887-6080)', 'Eduard Magazin',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>76</v>
       </c>
@@ -14688,12 +14990,15 @@
       <c r="P77" s="2">
         <v>1</v>
       </c>
-      <c r="R77" s="3" t="str">
+      <c r="Q77" s="42" t="s">
+        <v>1896</v>
+      </c>
+      <c r="S77" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kuglački klub Liburnija',  76, '023/633-074','','','01388797', '12853339056','13000258', '0102963', 'Petar Ugarković (091/528-93-33)', 'Čedo Alić',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>77</v>
       </c>
@@ -14740,12 +15045,15 @@
       <c r="P78" s="2">
         <v>1</v>
       </c>
-      <c r="R78" s="3" t="str">
+      <c r="Q78" s="37" t="s">
+        <v>1880</v>
+      </c>
+      <c r="S78" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Hrvački klub Zadar',  77, '023/332-680','','023/332-680','02750104', '00749599062','13001288', '0177980', 'Vladimir Menčik (098/957-97-49)', 'Mirela Menčik',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>78</v>
       </c>
@@ -14788,12 +15096,15 @@
       <c r="P79" s="2">
         <v>1</v>
       </c>
-      <c r="R79" s="3" t="str">
+      <c r="Q79" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S79" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo Športske Rekreacije Dite zadarsko',  78, '023/250-275','','','025559889', '36453025190','13001143', '0101911', 'Venci Longin (098/175-01-40)', '',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>79</v>
       </c>
@@ -14838,12 +15149,15 @@
       <c r="P80" s="2">
         <v>1</v>
       </c>
-      <c r="R80" s="3" t="str">
+      <c r="Q80" s="37" t="s">
+        <v>1909</v>
+      </c>
+      <c r="S80" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Odbojkaški klub Arbanasi',  79, '023/250-120','','023/254-020','01802020', '10199002785','13000703', '0112272', 'Karlo Lisica (091/799-62479', '',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>80</v>
       </c>
@@ -14890,12 +15204,15 @@
       <c r="P81" s="2">
         <v>1</v>
       </c>
-      <c r="R81" s="3" t="str">
+      <c r="Q81" s="37" t="s">
+        <v>1916</v>
+      </c>
+      <c r="S81" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub daljinskog plivanja Donat',  80, '023/300-444','','023/300-444','01944835', '18693109162','13000784', '0120399', 'Hrvoje Bajlo (091/564-02-12)', 'Siniša Pezelj',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>81</v>
       </c>
@@ -14942,12 +15259,15 @@
       <c r="P82" s="2">
         <v>1</v>
       </c>
-      <c r="R82" s="3" t="str">
+      <c r="Q82" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S82" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kiteboarding udruga Adrenalin',  81, '023/334-414','','023/334-414','01477951', '50228536500','13000437', '0188755', 'Damir Veledar (099/513-42-18)', 'Maria Veledar',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>82</v>
       </c>
@@ -14994,12 +15314,15 @@
       <c r="P83" s="2">
         <v>1</v>
       </c>
-      <c r="R83" s="3" t="str">
+      <c r="Q83" s="37" t="s">
+        <v>1881</v>
+      </c>
+      <c r="S83" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub jedrenja na dasci Fortunal',  82, '023/334-414','','023/334-414','01285122', '72975768959','13000201', '0188763', 'Damir Veledar (091/513-42-18)', 'Marinko Miočić (098/685-502)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>83</v>
       </c>
@@ -15044,12 +15367,15 @@
       <c r="P84" s="2">
         <v>1</v>
       </c>
-      <c r="R84" s="3" t="str">
+      <c r="Q84" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S84" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo za športsku rekreaciju Relaks',  83, '023/326-225','','023/326-225','00769118', '72633484931','13000018', '0151453', 'Katja Pijaca (091/509-28-75)', '',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>84</v>
       </c>
@@ -15096,12 +15422,15 @@
       <c r="P85" s="2">
         <v>1</v>
       </c>
-      <c r="R85" s="3" t="str">
+      <c r="Q85" s="37" t="s">
+        <v>1933</v>
+      </c>
+      <c r="S85" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski klub za skokove u vodu Arno',  84, '023/313-192','','023/313-192','2043025', '56403849809','13000864', '0151652', 'Veljko Bubić', 'Arno Longin (098/171-30-97)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>85</v>
       </c>
@@ -15146,12 +15475,15 @@
       <c r="P86" s="2">
         <v>1</v>
       </c>
-      <c r="R86" s="3" t="str">
+      <c r="Q86" s="37" t="s">
+        <v>1889</v>
+      </c>
+      <c r="S86" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kickboxing klub Sv. Krševan',  85, '023/318-401','','','01774433', '08024726070','13000392', '0192946', 'Neenad Mitrović (098/924-98-42)', 'Jurica Kvartuč',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>86</v>
       </c>
@@ -15196,12 +15528,15 @@
       <c r="P87" s="2">
         <v>1</v>
       </c>
-      <c r="R87" s="3" t="str">
+      <c r="Q87" s="42" t="s">
+        <v>1749</v>
+      </c>
+      <c r="S87" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boksački klub Sv. Krševan',  86, '023/318-401','','','01433806', '97042242606','13000392', '0192959', 'Nenad Mitrović (098/924-98-42)', 'Jurica Kvartuč',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>87</v>
       </c>
@@ -15248,12 +15583,15 @@
       <c r="P88" s="2">
         <v>1</v>
       </c>
-      <c r="R88" s="3" t="str">
+      <c r="Q88" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S88" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Varoš',  87, '023/327-372','','023/327-372','02561425', '29063643242','13001159', '0189548', 'Marko Jurin (099/736-85-49)', 'Marko Vukić (099/249-81-81)',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>88</v>
       </c>
@@ -15300,12 +15638,15 @@
       <c r="P89" s="2">
         <v>1</v>
       </c>
-      <c r="R89" s="3" t="str">
+      <c r="Q89" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S89" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Sonik Puntamika',  88, '023/335-735','','023/335-735','01373137', '94165900313','13000189', '0125060', 'Mirko Jošić (091/121-10-65)', 'Pero Perić (091/547-73-72)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>89</v>
       </c>
@@ -15348,12 +15689,15 @@
       <c r="P90" s="2">
         <v>1</v>
       </c>
-      <c r="R90" s="3" t="str">
+      <c r="Q90" s="42" t="s">
+        <v>1889</v>
+      </c>
+      <c r="S90" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kickboxing klub Sv. Zoilo',  89, '','','','02726050', '76521889373','13001245', '0164440', 'Tomislav Torić (095/8000-48-86)', 'Jure Čačić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>90</v>
       </c>
@@ -15392,12 +15736,15 @@
       <c r="P91" s="2">
         <v>1</v>
       </c>
-      <c r="R91" s="3" t="str">
+      <c r="Q91" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S91" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Euforija',  90, '','','','04044169', '15855531924','13001470', '0248415', 'Marina Tomas (098/6500-07)', 'Tina KAravida ((099/310-14-48)',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>91</v>
       </c>
@@ -15440,12 +15787,15 @@
       <c r="P92" s="2">
         <v>1</v>
       </c>
-      <c r="R92" s="3" t="str">
+      <c r="Q92" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S92" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo za športsku rekreaciju Hula-hop',  91, '023/323-552','','','04085558', '24161670928','13001484', '0251998', 'Radojka Antić (098/42-97-61)', '',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>92</v>
       </c>
@@ -15492,12 +15842,15 @@
       <c r="P93" s="2">
         <v>1</v>
       </c>
-      <c r="R93" s="3" t="str">
+      <c r="Q93" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S93" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Košarkaški klub Zara',  92, '023/341-286','','023/236-384','04060938', '97422202178','13001477', '0249667', 'Marin Vrsaljko (098/221-448)', 'Ana Vrsaljko',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>93</v>
       </c>
@@ -15538,12 +15891,15 @@
       <c r="P94" s="2">
         <v>1</v>
       </c>
-      <c r="R94" s="3" t="str">
+      <c r="Q94" s="42" t="s">
+        <v>1749</v>
+      </c>
+      <c r="S94" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boksački klub Dijagora',  93, '023/316-114','','','01167513', '53085011457','13000608', '', 'Denis Gregov (091/907-23-81)', '',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>94</v>
       </c>
@@ -15580,12 +15936,15 @@
       <c r="P95" s="2">
         <v>1</v>
       </c>
-      <c r="R95" s="3" t="str">
+      <c r="Q95" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S95" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski centar Višnjik d.o.o.',  94, '023/449-860','','023/302-402','01759418', '79086303924','', '', 'Denis Karlović (098/369-515)', '',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('16.07.2013', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>95</v>
       </c>
@@ -15632,12 +15991,15 @@
       <c r="P96" s="2">
         <v>1</v>
       </c>
-      <c r="R96" s="3" t="str">
+      <c r="Q96" s="37" t="s">
+        <v>1893</v>
+      </c>
+      <c r="S96" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ženski košarkaški klub Zadar',  95, '023/350-356','','023/350-355','00516376', '30110621801','13000159', '0117756', 'Branimir Perićić (095/910-71-79)', 'Josipa Sesar',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>96</v>
       </c>
@@ -15684,12 +16046,15 @@
       <c r="P97" s="2">
         <v>1</v>
       </c>
-      <c r="R97" s="3" t="str">
+      <c r="Q97" s="42" t="s">
+        <v>1881</v>
+      </c>
+      <c r="S97" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Jedriličarski klub Sv. Krševan',  96, '023/231-679','','023/231-679','01461834', '63499196019','130100112', '0130435', 'Edo Fantela (098/940-417-72)', 'Nives Letinić',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>97</v>
       </c>
@@ -15726,12 +16091,15 @@
       <c r="P98" s="2">
         <v>1</v>
       </c>
-      <c r="R98" s="3" t="str">
+      <c r="Q98" s="42" t="s">
+        <v>1886</v>
+      </c>
+      <c r="S98" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Karate  klub Zadar',  97, '','','','', '67131312087','13000302', '', 'Goran Glavan (098/272-848)', '',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>98</v>
       </c>
@@ -15774,12 +16142,15 @@
       <c r="P99" s="2">
         <v>1</v>
       </c>
-      <c r="R99" s="3" t="str">
+      <c r="Q99" s="37" t="s">
+        <v>1884</v>
+      </c>
+      <c r="S99" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ju jitsu klub Zadar',  98, '','','','01662015', '18212327717','13000618', '0132381', 'Damir Šalina (091/721-47-37)', 'Vedran Šetka',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>99</v>
       </c>
@@ -15824,12 +16195,15 @@
       <c r="P100" s="2">
         <v>1</v>
       </c>
-      <c r="R100" s="3" t="str">
+      <c r="Q100" s="37" t="s">
+        <v>1884</v>
+      </c>
+      <c r="S100" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ju jitsu klub Donat',  99, '023/214-848','','','02515199', '19634543545','13001125', '0205449', 'Saša Stipanić (099/530-04-78)', 'Samir Sedić (098/429-863)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="101" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>100</v>
       </c>
@@ -15872,12 +16246,15 @@
       <c r="P101" s="2">
         <v>1</v>
       </c>
-      <c r="R101" s="3" t="str">
+      <c r="Q101" s="42" t="s">
+        <v>1886</v>
+      </c>
+      <c r="S101" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boksački klub Zlatna Rukavica',  100, '','','','02317460', '09173545142','13000977', '0127932', 'Šime Filipi (098/941-58-19)', 'Edi Milošević (095/395-84-98)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>101</v>
       </c>
@@ -15918,12 +16295,15 @@
       <c r="P102" s="2">
         <v>1</v>
       </c>
-      <c r="R102" s="3" t="str">
+      <c r="Q102" s="37" t="s">
+        <v>1750</v>
+      </c>
+      <c r="S102" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Body Building klub Hulk',  101, '','','','4010094', '62291466931','13001456', '', 'Zoran Tokić (095/819-91-92)', 'Viktor Begonja',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>102</v>
       </c>
@@ -15970,12 +16350,15 @@
       <c r="P103" s="2">
         <v>1</v>
       </c>
-      <c r="R103" s="3" t="str">
+      <c r="Q103" s="37" t="s">
+        <v>1951</v>
+      </c>
+      <c r="S103" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Taekwondo klub Plovanija',  102, '023/324-118','','023/312-235','02607867', '34802146621','13001187', '0140147', 'Antonio Čačić (098/928-94-56)', 'Danijela Sipina 095/9082610',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>103</v>
       </c>
@@ -16022,12 +16405,15 @@
       <c r="P104" s="2">
         <v>1</v>
       </c>
-      <c r="R104" s="3" t="str">
+      <c r="Q104" s="42" t="s">
+        <v>1875</v>
+      </c>
+      <c r="S104" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Gimnastički klub Zadar',  103, '023/250-120','','023/250-120','03155056', '86639247638','9537800000', '0112299', 'Magdalena Brković (095/391-38-05)', 'Saša Brković',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>104</v>
       </c>
@@ -16074,12 +16460,15 @@
       <c r="P105" s="2">
         <v>1</v>
       </c>
-      <c r="R105" s="3" t="str">
+      <c r="Q105" s="37" t="s">
+        <v>1891</v>
+      </c>
+      <c r="S105" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Konjički klub Epona',  104, '023/313-036','','023/313-036','01492152', '69853428287','13000460', '0273360', 'Edo Jelenković (099/673-71-06)', 'Marin Kožul',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>105</v>
       </c>
@@ -16122,12 +16511,15 @@
       <c r="P106" s="2">
         <v>1</v>
       </c>
-      <c r="R106" s="3" t="str">
+      <c r="Q106" s="42" t="s">
+        <v>1941</v>
+      </c>
+      <c r="S106" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Streljački klub Lovac',  105, '023/230-000','','0237220-797','03154815', '35307886697','13000324', '0140365', 'Danijel Telesmanić (091/226-21-00)', 'Arden Dražević',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>106</v>
       </c>
@@ -16168,12 +16560,15 @@
       <c r="P107" s="2">
         <v>1</v>
       </c>
-      <c r="R107" s="3" t="str">
+      <c r="Q107" s="42" t="s">
+        <v>1933</v>
+      </c>
+      <c r="S107" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub za skokove u vodu Zadar',  106, '','','','03429679', '71809427092','13000330', '0171087', 'Mirko Jurin (098/813-44-31)', '',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>107</v>
       </c>
@@ -16218,12 +16613,15 @@
       <c r="P108" s="2">
         <v>1</v>
       </c>
-      <c r="R108" s="3" t="str">
+      <c r="Q108" s="42" t="s">
+        <v>1923</v>
+      </c>
+      <c r="S108" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Rukometni klub Arbanasi',  107, '023/317-279','','','02378531', '91835955260','13001023', '0115934', 'Stipe Bjeliš (098/164-25-48)', 'Vatroslav Ivković',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>108</v>
       </c>
@@ -16264,12 +16662,15 @@
       <c r="P109" s="2">
         <v>1</v>
       </c>
-      <c r="R109" s="3" t="str">
+      <c r="Q109" s="37" t="s">
+        <v>1948</v>
+      </c>
+      <c r="S109" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Klub za športski ribolov Paprenica',  108, '','','','02647774', '73892282141','13001205', '', 'Josip-Pero Granić (098/961-74-74)', 'Ljubomir Čurković',to_date(NULLIF('01.01.2009', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>109</v>
       </c>
@@ -16314,12 +16715,15 @@
       <c r="P110" s="2">
         <v>1</v>
       </c>
-      <c r="R110" s="3" t="str">
+      <c r="Q110" s="37" t="s">
+        <v>1948</v>
+      </c>
+      <c r="S110" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski ribolovni klub Donat',  109, '023/233-766','','023/233-766','01432974', '03595482979','13000394', '0134892', 'Josip Gatara', 'Davorka Volarević',to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.07.2014', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>110</v>
       </c>
@@ -16366,12 +16770,15 @@
       <c r="P111" s="2">
         <v>1</v>
       </c>
-      <c r="R111" s="3" t="str">
+      <c r="Q111" s="37" t="s">
+        <v>1914</v>
+      </c>
+      <c r="S111" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Alpinistički klub Zadar',  110, '053/679-112','','053/679-112','02490463', '45680132118','13001106', '0151216', 'Jana Mijailović (095/827-29-43)', 'Natalija Andačić',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>111</v>
       </c>
@@ -16418,12 +16825,15 @@
       <c r="P112" s="2">
         <v>1</v>
       </c>
-      <c r="R112" s="3" t="str">
+      <c r="Q112" s="42" t="s">
+        <v>1909</v>
+      </c>
+      <c r="S112" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Odbojkaški klub Donat',  111, '023/327-265','','023/327-265','02217830', '23517960553','13000888', '0151445', 'Julja Kaleb (098/191-27-28)', 'Irena Kraljev Mesarić',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>112</v>
       </c>
@@ -16470,12 +16880,15 @@
       <c r="P113" s="2">
         <v>1</v>
       </c>
-      <c r="R113" s="3" t="str">
+      <c r="Q113" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S113" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Hrvatski nogometni klub Dalmatinac',  112, '023/300-002','','023/300-002','1472712', '73680202956','13000426', '0338503', 'Mile Vukoša (098/273-807)', 'Jurica Grgurović (091/380-51-55)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>113</v>
       </c>
@@ -16518,12 +16931,15 @@
       <c r="P114" s="2">
         <v>1</v>
       </c>
-      <c r="R114" s="3" t="str">
+      <c r="Q114" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S114" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga slijepih Zadarske Županije',  113, '023/250-546','','023/250-546','01075497', '85389451415','13000100', '0002348', 'Danijel Lončar (091/548-80-02)', 'Špiro Zrilić',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>114</v>
       </c>
@@ -16570,12 +16986,15 @@
       <c r="P115" s="2">
         <v>1</v>
       </c>
-      <c r="R115" s="3" t="str">
+      <c r="Q115" s="37" t="s">
+        <v>1945</v>
+      </c>
+      <c r="S115" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski savez gluhih Zadarske Županije',  114, '023/7213-442','','023/7213-442','04277708', '19460481165','13001350', '0285826', 'Natko Zelić', 'Miki Savić (091/764-70-47)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>115</v>
       </c>
@@ -16618,12 +17037,15 @@
       <c r="P116" s="2">
         <v>1</v>
       </c>
-      <c r="R116" s="3" t="str">
+      <c r="Q116" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S116" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Odbojkaški klub invalida Zadar',  115, '','','','02029715', '64155155306','13000838', '0062014', 'Ivan Bajlo (098/830-888)', 'Ante Baraba Knez (092/130-39-15)',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>116</v>
       </c>
@@ -16664,12 +17086,15 @@
       <c r="P117" s="2">
         <v>1</v>
       </c>
-      <c r="R117" s="3" t="str">
+      <c r="Q117" s="42" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S117" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kuglački klub invalida Dišpet',  116, '023/323-400','','023/323-777','02496259', '53410477438','13001122', '0188409', 'Dražen Žilić (091/503-62-88)', '',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>117</v>
       </c>
@@ -16716,12 +17141,15 @@
       <c r="P118" s="2">
         <v>1</v>
       </c>
-      <c r="R118" s="3" t="str">
+      <c r="Q118" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S118" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Plivački klub osoba s invaliditetom Sv. Nikola',  117, '023/323-400','','023/323-777','02430568', '38060095051','13001055', '0188384', 'Marin Raspović (099/578-40-46)', 'E. Šahinović (099/723-34-15)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>118</v>
       </c>
@@ -16766,12 +17194,15 @@
       <c r="P119" s="2">
         <v>1</v>
       </c>
-      <c r="R119" s="3" t="str">
+      <c r="Q119" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S119" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Stolnoteniski klub osoba s invaliditetom Sv. Krševan',  118, '023/323-400','','023-323-777','02336251', '33677229477','13001003', '0188392', 'Miroslav Barić (092/159-81-76)', '',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>119</v>
       </c>
@@ -16816,12 +17247,15 @@
       <c r="P120" s="2">
         <v>1</v>
       </c>
-      <c r="R120" s="3" t="str">
+      <c r="Q120" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S120" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Streljački klub osoba s invaliditetom Donat',  119, '023/323-400','','023/323-777','02180839', '76270962910','13000903', '0188417', 'Saša Grdović (098/417-401)', '',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>120</v>
       </c>
@@ -16868,12 +17302,15 @@
       <c r="P121" s="2">
         <v>1</v>
       </c>
-      <c r="R121" s="3" t="str">
+      <c r="Q121" s="42" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S121" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ribolovni klub osoba s invaliditetom Škartoc',  120, '023/323-400','','023/323-777','02093146', '89102866393','13000869', '0188433', 'Zoran Radić (099/250-76-66)', 'Elfad Šahinović (099/337-34-15)',to_date(NULLIF('01.01.2010', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="17">
         <v>121</v>
       </c>
@@ -16920,12 +17357,15 @@
       <c r="P122" s="2">
         <v>1</v>
       </c>
-      <c r="R122" s="3" t="str">
+      <c r="Q122" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S122" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Športski savez osoba s invaliditetom Zadarske županije',  121, '023/323-400','','023/323-777','02438887', '79668532267','130000929', '0188425', 'Saša Grdović (098/417-401)', 'Dražen Žilić',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>122</v>
       </c>
@@ -16970,12 +17410,15 @@
       <c r="P123" s="2">
         <v>1</v>
       </c>
-      <c r="R123" s="3" t="str">
+      <c r="Q123" s="37" t="s">
+        <v>1888</v>
+      </c>
+      <c r="S123" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kendo klub "Ouka"',  122, '098-665-752','','','01841823', '52434249167','13000740', '0329744', 'Marko Lukić (098/665-752)', 'Toni Tadić (099/835-05-08)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="17">
         <v>123</v>
       </c>
@@ -17022,12 +17465,15 @@
       <c r="P124" s="2">
         <v>1</v>
       </c>
-      <c r="R124" s="3" t="str">
+      <c r="Q124" s="37" t="s">
+        <v>1912</v>
+      </c>
+      <c r="S124" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Pikado Savez Zadarske župnije',  123, '023/316-400','','023/316-400','02939622', '82956603468','13001429', '0229577', 'Jure Jerak (091/433-23-66)', 'Ante Frleta (981/55-94-445)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="17">
         <v>124</v>
       </c>
@@ -17074,12 +17520,15 @@
       <c r="P125" s="2">
         <v>1</v>
       </c>
-      <c r="R125" s="3" t="str">
+      <c r="Q125" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S125" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga za "Down sindrom" Zadarske županije',  124, '023/636-603','','023/636-603','02238454', '93166915044','13000938', '0041759', 'Suzana Periša (095/906-3956)', 'Tanja Radman (099/218-74-90)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="17">
         <v>125</v>
       </c>
@@ -17122,12 +17571,15 @@
       <c r="P126" s="2">
         <v>1</v>
       </c>
-      <c r="R126" s="3" t="str">
+      <c r="Q126" s="37" t="s">
+        <v>1922</v>
+      </c>
+      <c r="S126" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ronilački klub 2 dive',  125, '','','','02349710', '712619004259','13001009', '0373883', 'Božidar Matković (091/500-0419)', 'Andrija Rogić (099/913-27-61)',to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2020', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" s="17">
         <v>126</v>
       </c>
@@ -17172,12 +17624,15 @@
       <c r="P127" s="2">
         <v>1</v>
       </c>
-      <c r="R127" s="3" t="str">
+      <c r="Q127" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S127" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Brodarica',  126, '091/191-22-01','','','02804808', '94926662660','13001323', '0190254', 'Hrvoje Medved (091/191-22-01)', 'Vladimir Gambiraža',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="17">
         <v>127</v>
       </c>
@@ -17216,12 +17671,15 @@
       <c r="P128" s="2">
         <v>1</v>
       </c>
-      <c r="R128" s="3" t="str">
+      <c r="Q128" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S128" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Zadar',  127, '092/304-67-63','','','4021096', '14511512212','13001460', '0283787', 'Roko Dujić (092-304-67-63)', '',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="17">
         <v>128</v>
       </c>
@@ -17264,12 +17722,15 @@
       <c r="P129" s="2">
         <v>1</v>
       </c>
-      <c r="R129" s="3" t="str">
+      <c r="Q129" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S129" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Petrčane',  128, '092/217-36-14','','','04027329', '09059794368','13001437', '0243751', 'Duje Stanišić (092/2173-614)', '',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="17">
         <v>129</v>
       </c>
@@ -17310,12 +17771,15 @@
       <c r="P130" s="2">
         <v>1</v>
       </c>
-      <c r="R130" s="3" t="str">
+      <c r="Q130" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S130" s="3" t="str">
         <f t="shared" si="1"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Osmijeh za-Dar',  129, '095/579-91-30','','','02434024', '69082966145','13001061', '0151554', 'Borut Gatara (095/ 579-91-30)', 'Sandra Profaca',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A131" s="17">
         <v>130</v>
       </c>
@@ -17356,12 +17820,15 @@
       <c r="P131" s="2">
         <v>1</v>
       </c>
-      <c r="R131" s="3" t="str">
-        <f t="shared" ref="R131:R160" si="2">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B131&amp;"',  "&amp;C131&amp;", '"&amp;D131&amp;"','"&amp;E131&amp;"','"&amp;F131&amp;"','"&amp;G131&amp;"', '"&amp;H131&amp;"','"&amp;I131&amp;"', '"&amp;J131&amp;"', '"&amp;K131&amp;"', '"&amp;L131&amp;"',to_date(NULLIF('"&amp;IF(M131="","",M131)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N131="","",N131)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O131="","",O131)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P131&amp;"');"</f>
+      <c r="Q131" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S131" s="3" t="str">
+        <f t="shared" ref="S131:S160" si="2">"insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number"&amp;", number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('"&amp;B131&amp;"',  "&amp;C131&amp;", '"&amp;D131&amp;"','"&amp;E131&amp;"','"&amp;F131&amp;"','"&amp;G131&amp;"', '"&amp;H131&amp;"','"&amp;I131&amp;"', '"&amp;J131&amp;"', '"&amp;K131&amp;"', '"&amp;L131&amp;"',to_date(NULLIF('"&amp;IF(M131="","",M131)&amp;"', ''),  'DD.MM.YYYY' ),to_date(NULLIF('"&amp;IF(N131="","",N131)&amp;"', ''),  'DD.MM.YYYY' ), to_date(NULLIF('"&amp;IF(O131="","",O131)&amp;"', ''),  'DD.MM.YYYY' ), '"&amp;P131&amp;"');"</f>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Novi Bokanjac',  130, '098/309-169','','','01696947', '74659664033','', '', 'Tomislav Dešpoja (098/309-164)', 'Antonio Zelić (091/238-52-48)  Kontakt osoba: Nikola Zrilić (098/843-593)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="17">
         <v>131</v>
       </c>
@@ -17408,12 +17875,15 @@
       <c r="P132" s="2">
         <v>1</v>
       </c>
-      <c r="R132" s="3" t="str">
+      <c r="Q132" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S132" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Kožino',  131, '023/343-421','','023/343-421','01882309', '32230828872','1300751', '0073504', 'Ivan Stručić (098-339-369)', 'Edi Tokić (091/2831-488)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="17">
         <v>132</v>
       </c>
@@ -17456,12 +17926,15 @@
       <c r="P133" s="2">
         <v>1</v>
       </c>
-      <c r="R133" s="3" t="str">
+      <c r="Q133" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S133" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Dragovoljac',  132, '023/315-546  ','098/330-095','023/315-546','4213157', '31607309251','0013001566', '0274802', 'Nino Rašin', 'Venci Kvartuč',to_date(NULLIF('', ''),  'DD.MM.YYYY' ),to_date(NULLIF('', ''),  'DD.MM.YYYY' ), to_date(NULLIF('', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="17">
         <v>133</v>
       </c>
@@ -17508,12 +17981,15 @@
       <c r="P134" s="2">
         <v>1</v>
       </c>
-      <c r="R134" s="3" t="str">
+      <c r="Q134" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S134" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Crvene kuće',  133, '095/905-28-81','','023/332-104','02640481', '05748485522','13001211', '0192491', 'Mate Marić (095/905-28-81)', 'Marko Tadić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('29.04.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="17">
         <v>134</v>
       </c>
@@ -17558,12 +18034,15 @@
       <c r="P135" s="2">
         <v>1</v>
       </c>
-      <c r="R135" s="3" t="str">
+      <c r="Q135" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S135" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo Bokanjac Zadar',  134, '023/221-575','','023/221-575','014228812', '32014543847','13000375', '0151485', 'Ivica Mrkić (095/910-04-52)', '',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="17">
         <v>135</v>
       </c>
@@ -17608,12 +18087,15 @@
       <c r="P136" s="2">
         <v>1</v>
       </c>
-      <c r="R136" s="3" t="str">
+      <c r="Q136" s="42" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S136" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Bili Brig',  135, '092/4067-090','','','02240530', '76996713327','13000834', '0346123', 'Mario Barišić', 'Šime Bašić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="17">
         <v>136</v>
       </c>
@@ -17658,12 +18140,15 @@
       <c r="P137" s="2">
         <v>1</v>
       </c>
-      <c r="R137" s="3" t="str">
+      <c r="Q137" s="42" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S137" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Društvo športske rekreacije Loptica',  136, '098/685-502','','','1736230', '17626883048','13000674', '0127961', 'Marinko Miočić', 'Ana Miočić',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="17">
         <v>137</v>
       </c>
@@ -17710,12 +18195,15 @@
       <c r="P138" s="2">
         <v>1</v>
       </c>
-      <c r="R138" s="3" t="str">
+      <c r="Q138" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S138" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga mladih Ista',  137, '098/967-04-72  ','097/791-05-72','','02345854', '33334206740','13000986', '0041734', 'Luka Kozulić (098/967-04-72)', 'Josipa Kozulić (098/913-44-13)',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="17">
         <v>138</v>
       </c>
@@ -17760,12 +18248,15 @@
       <c r="P139" s="2">
         <v>1</v>
       </c>
-      <c r="R139" s="3" t="str">
+      <c r="Q139" s="37" t="s">
+        <v>1746</v>
+      </c>
+      <c r="S139" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Zadarska plesna udruga Tornadele',  138, '091/356-97-72','','','02644703', '68451911353','13001195', '0164471', 'Helena Dobrović', 'Valentina Beneta',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A140" s="17">
         <v>139</v>
       </c>
@@ -17810,12 +18301,15 @@
       <c r="P140" s="2">
         <v>1</v>
       </c>
-      <c r="R140" s="3" t="str">
+      <c r="Q140" s="37" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S140" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kyudo udruga Yumi - Zadar',  139, '091/570-27-10','','','02489945', '33116958949','09000455', '0255149', 'Goran Blažević (091/570-27-10)', 'Alen Lonić (099/217-78-97)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="17">
         <v>140</v>
       </c>
@@ -17862,12 +18356,15 @@
       <c r="P141" s="2">
         <v>1</v>
       </c>
-      <c r="R141" s="3" t="str">
+      <c r="Q141" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S141" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Ženski nogometni klub Donat',  140, '098/429-608','','023/312-598','4401352', '56219903028','13001655', '0339839', 'Edvin Šimunov (098/429-608)', 'Doris Kalmeta (099/305-25-25)',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A142" s="17">
         <v>141</v>
       </c>
@@ -17914,12 +18411,15 @@
       <c r="P142" s="2">
         <v>1</v>
       </c>
-      <c r="R142" s="3" t="str">
+      <c r="Q142" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S142" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Bili Brig',  141, '023/778791','','023/778791','02556472', '93488686922','13001133', '0308611', 'Josip Lončar (091/161-37-04)', 'Marko Jurjević Škopinić (098/966-52-77)',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" s="17">
         <v>142</v>
       </c>
@@ -17966,12 +18466,15 @@
       <c r="P143" s="2">
         <v>1</v>
       </c>
-      <c r="R143" s="3" t="str">
+      <c r="Q143" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S143" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Plovanija',  142, '023/231-755','','023/231-755','02285690', '66570453161','13000980', '0073580', 'Martin Baričević (091/579-3351)', 'Željko Skukan (098/212-235)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="17">
         <v>143</v>
       </c>
@@ -18016,12 +18519,15 @@
       <c r="P144" s="2">
         <v>1</v>
       </c>
-      <c r="R144" s="3" t="str">
+      <c r="Q144" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S144" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Voštarnica',  143, '098/962-29-18','','','04276337', '19610029717','13001609', '0283228', 'Šime Erlić (098/962-29-18)', 'Ivan Erceg',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="17">
         <v>144</v>
       </c>
@@ -18064,12 +18570,15 @@
       <c r="P145" s="2">
         <v>1</v>
       </c>
-      <c r="R145" s="3" t="str">
+      <c r="Q145" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S145" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Ploča',  144, '091/575-83-76','','','2264218', '60049621539','13000965', '', 'Željko Gravić  (091/575-83-76)', 'Marko Pilipović',to_date(NULLIF('01.01.2007', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A146" s="17">
         <v>145</v>
       </c>
@@ -18116,12 +18625,15 @@
       <c r="P146" s="2">
         <v>1</v>
       </c>
-      <c r="R146" s="3" t="str">
+      <c r="Q146" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S146" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Stanovi',  145, '023/318-339','','023/318-339','01818686', '98871200553','13000708', '0243756', 'Toni Lovrić (095/557-52-42)', 'Luka Zubčić (091/731-32-28)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="17">
         <v>146</v>
       </c>
@@ -18166,12 +18678,15 @@
       <c r="P147" s="2">
         <v>1</v>
       </c>
-      <c r="R147" s="3" t="str">
+      <c r="Q147" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S147" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Sv. Ante',  146, '095/381-37-10','','','01375687', '47146690100','13000080', '0342073', 'Krešimir Zrilić', 'Ante Vukorepa',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="17">
         <v>147</v>
       </c>
@@ -18218,12 +18733,15 @@
       <c r="P148" s="2">
         <v>1</v>
       </c>
-      <c r="R148" s="3" t="str">
+      <c r="Q148" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S148" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Zapuntel',  147, '023/316-526  ','095/912-11-94','','02261260', '29723903297','13000959', '0103986', 'Neven Petrović (095/912-11-94)', 'Marin Petričić (098/1853-919)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A149" s="17">
         <v>148</v>
       </c>
@@ -18270,12 +18788,15 @@
       <c r="P149" s="2">
         <v>1</v>
       </c>
-      <c r="R149" s="3" t="str">
+      <c r="Q149" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S149" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Mala Rava',  148, '098/922-86-83  ','091/144-02-48','','02211483', '16335604791','13000935', '0186962', 'Vladimir Gambiraža (098/929-08-31)', 'Danijel Simičić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" s="17">
         <v>149</v>
       </c>
@@ -18322,12 +18843,15 @@
       <c r="P150" s="2">
         <v>1</v>
       </c>
-      <c r="R150" s="3" t="str">
+      <c r="Q150" s="42" t="s">
+        <v>1923</v>
+      </c>
+      <c r="S150" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Rukometni klub Zadar 2013',  149, '095/860-92-01','','023/241909','04113225', '41853702244','13001506', '0254317', 'Anđelo Šare (095/ 860-92-01)', 'Barbara Kardum',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="151" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="17">
         <v>150</v>
       </c>
@@ -18372,12 +18896,15 @@
       <c r="P151" s="2">
         <v>1</v>
       </c>
-      <c r="R151" s="3" t="str">
+      <c r="Q151" s="42" t="s">
+        <v>1881</v>
+      </c>
+      <c r="S151" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Jedriličarski klub Punta Bajlo',  150, '098/369-318','','','1602861', '69933257401','13000560', '0136670', 'Mladen Bajlo', 'Darko Smrkinić',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="17">
         <v>151</v>
       </c>
@@ -18422,12 +18949,15 @@
       <c r="P152" s="2">
         <v>1</v>
       </c>
-      <c r="R152" s="3" t="str">
+      <c r="Q152" s="42" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S152" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Plivački klub osoba s invaliditetom Frogo',  151, '095/359-70-55','','','04395549', '42484305521','13001652', '0331558', 'Sanja Sedić', 'Silva Žabo',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="153" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="17">
         <v>152</v>
       </c>
@@ -18474,12 +19004,15 @@
       <c r="P153" s="2">
         <v>1</v>
       </c>
-      <c r="R153" s="3" t="str">
+      <c r="Q153" s="37" t="s">
+        <v>1913</v>
+      </c>
+      <c r="S153" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Hrvatsko planinarsko društvo Zavrata',  152, '091/600-00-31  ','098/981-73-22','','04336593', '02298099199','13001627', '0342260', 'Nikola Stilinović', 'Ante Pušić',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="154" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" s="17">
         <v>153</v>
       </c>
@@ -18524,12 +19057,15 @@
       <c r="P154" s="2">
         <v>1</v>
       </c>
-      <c r="R154" s="3" t="str">
+      <c r="Q154" s="37" t="s">
+        <v>1678</v>
+      </c>
+      <c r="S154" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Udruga Hrvatskih vojnih invalida domovinskog rata - Zadar',  153, '023/323-400','','023/3323-777','03926281', '07666214502','13000103', '0073669', 'Ivica Arbanas (099/222-75-00)', 'Denis Simičić (099/223-36-81)',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="155" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A155" s="17">
         <v>154</v>
       </c>
@@ -18576,12 +19112,15 @@
       <c r="P155" s="2">
         <v>1</v>
       </c>
-      <c r="R155" s="3" t="str">
+      <c r="Q155" s="37" t="s">
+        <v>1959</v>
+      </c>
+      <c r="S155" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Aero klub Zadar',  154, '023/322-355','','023/322-355','03154823', '49059640059','13000131', '0073725', 'Bjanka Pavin (098/273-809)', 'Velid Jakupović (091/523-85-98)',to_date(NULLIF('01.01.2013', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2017', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="17">
         <v>155</v>
       </c>
@@ -18628,12 +19167,15 @@
       <c r="P156" s="2">
         <v>1</v>
       </c>
-      <c r="R156" s="3" t="str">
+      <c r="Q156" s="42" t="s">
+        <v>1751</v>
+      </c>
+      <c r="S156" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Boćarski Športski klub Zadar',  155, '023/214-093','','023/214-093','03450848', '03836929990','13000253', '0217137', 'Milivoj Colić (098/196-27-65)', 'Šime Buterin (098/175-14-97)',to_date(NULLIF('01.01.2008', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ), to_date(NULLIF('01.01.1996', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A157" s="17">
         <v>156</v>
       </c>
@@ -18680,12 +19222,15 @@
       <c r="P157" s="2">
         <v>1</v>
       </c>
-      <c r="R157" s="3" t="str">
+      <c r="Q157" s="42" t="s">
+        <v>1961</v>
+      </c>
+      <c r="S157" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('GRADSKI OGRANAK UDRUGE HRVATSKIH DRAGOVOLJACA DOMOVINSKOG RATA GRADA ZADRA',  156, '023/315-546','','023/315-546','4213157', '31607309251','0013001566', '0274802', 'Nino Rašin (091/524-30-72)', 'Venci Kvartuč (098/330-095)',to_date(NULLIF('01.01.2014', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2018', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="158" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="17">
         <v>157</v>
       </c>
@@ -18728,12 +19273,15 @@
       <c r="P158" s="2">
         <v>1</v>
       </c>
-      <c r="R158" s="3" t="str">
+      <c r="Q158" s="37" t="s">
+        <v>1906</v>
+      </c>
+      <c r="S158" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Malonogometni klub Brodarica',  157, '098/-990-73-99','','','2458594', '08244505631','13001082', '', 'Hrvoje Medved  (098/-990-73-99)', 'Denis Virovac',to_date(NULLIF('01.01.2012', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2016', ''),  'DD.MM.YYYY' ), to_date(NULLIF('12.10.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A159" s="17">
         <v>158</v>
       </c>
@@ -18778,12 +19326,15 @@
       <c r="P159" s="2">
         <v>1</v>
       </c>
-      <c r="R159" s="3" t="str">
+      <c r="Q159" s="42" t="s">
+        <v>1889</v>
+      </c>
+      <c r="S159" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Kick-Boxing klub Fight Factory',  158, '091/7859200','','','4489071', '13014500930','13001699', '0354938', 'Željko Dilber', 'Tajnik: Denis Kardum / Ovlaštena osoba: Ante Verunica (091/7859200)',to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2019', ''),  'DD.MM.YYYY' ), to_date(NULLIF('08.12.2015', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="17">
         <v>159</v>
       </c>
@@ -18826,7 +19377,10 @@
       <c r="P160" s="2">
         <v>1</v>
       </c>
-      <c r="R160" s="3" t="str">
+      <c r="Q160" s="42" t="s">
+        <v>1913</v>
+      </c>
+      <c r="S160" s="3" t="str">
         <f t="shared" si="2"/>
         <v>insert into diskobolos.member_register (name, location_id, phone1, phone2, fax, identification_number, oib, register_number, number_of_non_profit_org, chairman, secretary, date_from, date_to, registration_date, membership_category) values ('Planinarsko društvo Sveti Bernard',  159, '091/761 25 39','','','02851245', '04176260415','13001362', '0219130', 'Neven Zrilić (091/761-25-39 )', 'Šime Jukić (095/910-25-44)',to_date(NULLIF('01.01.2011', ''),  'DD.MM.YYYY' ),to_date(NULLIF('01.01.2015', ''),  'DD.MM.YYYY' ), to_date(NULLIF('', ''),  'DD.MM.YYYY' ), '1');</v>
       </c>
@@ -24009,7 +24563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24054,7 +24608,7 @@
         <v>1760</v>
       </c>
       <c r="C5" s="25" t="str">
-        <f t="shared" ref="C2:C116" si="0">"insert into diskobolos.sport (name) values ( '"&amp;A5&amp;"');"</f>
+        <f t="shared" ref="C5:C116" si="0">"insert into diskobolos.sport (name) values ( '"&amp;A5&amp;"');"</f>
         <v>insert into diskobolos.sport (name) values ( 'AMERIČKI NOGOMET (FOOTBALL)');</v>
       </c>
     </row>

</xml_diff>